<commit_message>
clean-up and new samples
</commit_message>
<xml_diff>
--- a/ExcelDataReaderApp/Customers.xlsx
+++ b/ExcelDataReaderApp/Customers.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OED\Dotnetland\VS2019\WorkingWithExcel\EPPlus1\02-ReadWorkbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OED\DotnetLand\VS2022\closet-code\ExcelDataReaderApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
+    <sheet name="Customers1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="312">
   <si>
     <t>Company</t>
   </si>
@@ -1314,25 +1315,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>126</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>130</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>136</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>139</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -2252,7 +2253,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>145</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -2298,7 +2299,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>154</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>157</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>167</v>
       </c>
@@ -2436,7 +2437,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -2459,7 +2460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>178</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>181</v>
       </c>
@@ -2528,7 +2529,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>184</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>187</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>199</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>202</v>
       </c>
@@ -2689,7 +2690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>206</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>211</v>
       </c>
@@ -2735,7 +2736,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>218</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>222</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>225</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>238</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>241</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>244</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>247</v>
       </c>
@@ -2988,7 +2989,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>251</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>254</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>257</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>260</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>263</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>266</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>269</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>273</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>276</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>279</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>282</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>285</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>288</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>291</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>294</v>
       </c>
@@ -3333,7 +3334,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>297</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>300</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>303</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>306</v>
       </c>
@@ -3425,7 +3426,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>309</v>
       </c>
@@ -3446,6 +3447,125 @@
       </c>
       <c r="G92">
         <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43945.831903635677</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43408.0625</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43285.541666666664</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>